<commit_message>
Conteo de vectores soporte.
Se verificaron los resultados de los parámetros y se hizo el conteo de vectores soporte
</commit_message>
<xml_diff>
--- a/Resultados_30Jun2020.xlsx
+++ b/Resultados_30Jun2020.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riemannruiz\Documents\GitHub\Proyecto-Mape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97E79D0-DEEF-40F0-80F2-0DB240F0754A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E511940-42A0-4BA1-96E6-1EFB851F048B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{FE3B9146-550C-4A67-8FA9-529536DD3D59}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{FE3B9146-550C-4A67-8FA9-529536DD3D59}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Resultados1" sheetId="1" r:id="rId1"/>
+    <sheet name="Resultados2" sheetId="2" r:id="rId2"/>
+    <sheet name="Resultados3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="22">
   <si>
     <t>Resultados</t>
   </si>
@@ -86,11 +88,20 @@
   <si>
     <t>parámetro no válido para ese kernel</t>
   </si>
+  <si>
+    <t>Número de vectores soporte</t>
+  </si>
+  <si>
+    <t>Vectores soporte</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -131,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -143,11 +154,306 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -290,19 +596,59 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C1C7723-8A9C-4D3F-8CE4-3FA0531D0B70}" name="Tabla1" displayName="Tabla1" ref="A3:J19" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C1C7723-8A9C-4D3F-8CE4-3FA0531D0B70}" name="Tabla1" displayName="Tabla1" ref="A3:J19" totalsRowShown="0" dataDxfId="22">
   <autoFilter ref="A3:J19" xr:uid="{93EB431F-AEED-4B74-85F6-B4EF002C44F9}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{3EC4ED12-868F-4CF4-AB9E-08A6B5E56E47}" name="Formulación"/>
     <tableColumn id="2" xr3:uid="{41BA13DF-04DD-4FDB-B79F-5F159E436BE3}" name="Función"/>
     <tableColumn id="3" xr3:uid="{085C5D2B-EAD3-44AD-B543-0FAC9965D6C5}" name="Kernel"/>
-    <tableColumn id="4" xr3:uid="{485FE0BE-6A27-4B4F-98C4-824930AFA812}" name="epsilon" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{485FE0BE-6A27-4B4F-98C4-824930AFA812}" name="epsilon" dataDxfId="21"/>
     <tableColumn id="5" xr3:uid="{E2017637-4C19-4114-81B1-E9223BAFD6CF}" name="c"/>
-    <tableColumn id="6" xr3:uid="{4B03B6C0-3032-4DC7-A0A9-B5DB0D6CE048}" name="v" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{A32A3CB0-F02D-4C54-B05C-5C6DD08F45C4}" name="gamma" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{9DC40533-1215-403C-8176-3D5B80A4D94B}" name="lck" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{5551318E-732F-4397-9626-1E13D518249F}" name="mape" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{1BA62D5B-9ECA-40AE-ACA4-2A7F35AA3F0F}" name="rmse" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{4B03B6C0-3032-4DC7-A0A9-B5DB0D6CE048}" name="v" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{A32A3CB0-F02D-4C54-B05C-5C6DD08F45C4}" name="gamma" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{9DC40533-1215-403C-8176-3D5B80A4D94B}" name="lck" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{5551318E-732F-4397-9626-1E13D518249F}" name="mape" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{1BA62D5B-9ECA-40AE-ACA4-2A7F35AA3F0F}" name="rmse" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FDC8E0B3-3226-46F0-B7DB-3626A23A1A44}" name="Tabla13" displayName="Tabla13" ref="A3:K19" totalsRowShown="0" dataDxfId="15">
+  <autoFilter ref="A3:K19" xr:uid="{314627D3-3F2B-4E78-96B5-766261AE39CA}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{7006A432-5D38-446E-8E39-96F943F68AF8}" name="Formulación"/>
+    <tableColumn id="2" xr3:uid="{956F3056-2479-42E8-8EFF-47B727F7C63D}" name="Función"/>
+    <tableColumn id="3" xr3:uid="{BCFEFCCF-40E9-43E5-8534-AD7D86F90BDB}" name="Kernel"/>
+    <tableColumn id="4" xr3:uid="{786067BE-8FC3-49A1-A3CE-CC0EF18BD52D}" name="epsilon" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{4AFB6C77-1D1E-4F0F-A01D-E04473629F9A}" name="c"/>
+    <tableColumn id="6" xr3:uid="{F6A2ECA7-C7A8-44B1-9E44-960EBC2D91AA}" name="v" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{C993A36D-CE55-4BA0-850E-553C1FB97E4F}" name="gamma" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{2EF37E22-F6CD-41C9-ADE2-E0139CFEDF9E}" name="lck" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{04CA0B35-D8EF-4EF7-B0BA-886BF96DD56D}" name="mape" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{97BD8495-EC38-47F7-B9E8-B2685E29F428}" name="rmse" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{54D34BFE-AB2E-4C34-BFD0-01830491F500}" name="Número de vectores soporte" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B7DA42D8-E12B-4CF7-A7AF-7622514E6A13}" name="Tabla134" displayName="Tabla134" ref="A3:K19" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A3:K19" xr:uid="{E0D41551-4D5E-42F5-BDBA-20D449CE6159}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{7B8B6D1E-65DF-450B-823E-DFAA74D78AF2}" name="Formulación"/>
+    <tableColumn id="2" xr3:uid="{D348B447-9DED-4CFB-A9E1-25DC4D4B9710}" name="Función"/>
+    <tableColumn id="3" xr3:uid="{ED44B7C7-4414-4BDA-BA25-1C2638049DFC}" name="Kernel"/>
+    <tableColumn id="4" xr3:uid="{6717FBDC-8DDB-4EB9-9F07-2FDF40F7AF5A}" name="epsilon" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{08C2A8E9-A9EC-4257-88B8-531CB60CCAC0}" name="c"/>
+    <tableColumn id="6" xr3:uid="{EB943433-53D7-4E54-9D02-C910436167E3}" name="v" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{B087ABF6-1EF2-4304-AE6E-36BDD50437A5}" name="gamma" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{3D00195F-4006-431C-A91B-282B3B8AC8D8}" name="lck" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{CE0CFFDA-DDA4-4D55-A4F4-E5F1D433A612}" name="mape" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{AF35A72C-5D0E-4932-B9B8-BB69850A1F9C}" name="rmse" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{472DA0E9-4141-4F91-87E8-0839A502CA06}" name="Vectores soporte" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -607,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1AC3C6-783D-41B9-9D49-E92EF6A6462C}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1178,4 +1524,1218 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903D8473-9875-4E40-8A61-B419802F229E}">
+  <dimension ref="A3:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="11" max="11" width="25.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>12.74321958</v>
+      </c>
+      <c r="F4" s="1">
+        <v>52.859676589999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>96.838433699999996</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.61568851999999996</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1.1990000000000001E-6</v>
+      </c>
+      <c r="J4" s="5">
+        <v>3.2630000000000002E-14</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1">
+        <v>66.649433500000001</v>
+      </c>
+      <c r="G5" s="1">
+        <v>84.867683600000007</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.02898891E-2</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1.1990000000000001E-6</v>
+      </c>
+      <c r="J5" s="5">
+        <v>3.2630000000000002E-14</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1">
+        <v>17.470003340000002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>12.93364319</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45.791012799999997</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2.2411222899999999</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.52154887000000005</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1.413E-14</v>
+      </c>
+      <c r="J6" s="5">
+        <v>3.2470000000000002E-29</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.0897436200000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>32.140378509999998</v>
+      </c>
+      <c r="F7" s="1">
+        <v>72.052134280000004</v>
+      </c>
+      <c r="G7" s="1">
+        <v>6.6573657500000003</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.37023394999999998</v>
+      </c>
+      <c r="I7" s="5">
+        <v>3.8000000000000002E-14</v>
+      </c>
+      <c r="J7" s="5">
+        <v>3.7190000000000001E-28</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8" s="1">
+        <v>25.189794970000001</v>
+      </c>
+      <c r="G8" s="1">
+        <v>54.566755100000002</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.59093600999999996</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1.7549999999999999E-6</v>
+      </c>
+      <c r="J8" s="5">
+        <v>5.259E-14</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>30.235382269999999</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>76.554354320000002</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.92326025</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1.7549999999999999E-6</v>
+      </c>
+      <c r="J9" s="5">
+        <v>5.259E-14</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.20799965000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>17.013050060000001</v>
+      </c>
+      <c r="F10" s="1">
+        <v>92.382394430000005</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.9952725299999998</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.37444251000000001</v>
+      </c>
+      <c r="I10" s="5">
+        <v>3.5180000000000001E-14</v>
+      </c>
+      <c r="J10" s="5">
+        <v>3.5580000000000001E-28</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1">
+        <v>17.929191589999999</v>
+      </c>
+      <c r="E11" s="1">
+        <v>69.986283319999998</v>
+      </c>
+      <c r="F11" s="1">
+        <v>35.277896339999998</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2.9669982699999999</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.90833008999999998</v>
+      </c>
+      <c r="I11" s="5">
+        <v>4.5360000000000002E-14</v>
+      </c>
+      <c r="J11" s="5">
+        <v>3.6339999999999998E-28</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>29.42410726</v>
+      </c>
+      <c r="F12" s="1">
+        <v>65.093202829999996</v>
+      </c>
+      <c r="G12" s="1">
+        <v>99.776767070000005</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1.1990000000000001E-6</v>
+      </c>
+      <c r="J12" s="5">
+        <v>3.2630000000000002E-14</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>50.281356850000002</v>
+      </c>
+      <c r="F13" s="1">
+        <v>28.03195152</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2.9069904800000002</v>
+      </c>
+      <c r="H13" s="1">
+        <v>5.0691739999999999E-2</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1.3469999999999999E-8</v>
+      </c>
+      <c r="J13" s="5">
+        <v>5.4320000000000001E-17</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14" s="1">
+        <v>98.218970850000005</v>
+      </c>
+      <c r="G14" s="1">
+        <v>26.76397291</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1.54E-13</v>
+      </c>
+      <c r="J14" s="5">
+        <v>7.9939999999999996E-27</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1">
+        <v>17.179269420000001</v>
+      </c>
+      <c r="E15" s="1">
+        <v>13.20003021</v>
+      </c>
+      <c r="F15" s="1">
+        <v>36.077645130000001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>100</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.41953826999999999</v>
+      </c>
+      <c r="I15" s="5">
+        <v>5.3029999999999997E-13</v>
+      </c>
+      <c r="J15" s="5">
+        <v>1.1120000000000001E-25</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>97.951985140000005</v>
+      </c>
+      <c r="F16" s="1">
+        <v>41.865225700000003</v>
+      </c>
+      <c r="G16" s="1">
+        <v>59.191153069999999</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.50026252000000004</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1.173E-7</v>
+      </c>
+      <c r="J16" s="5">
+        <v>1.856E-16</v>
+      </c>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>48.868004130000003</v>
+      </c>
+      <c r="F17" s="1">
+        <v>97.960398749999996</v>
+      </c>
+      <c r="G17" s="1">
+        <v>70.28819627</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.48970525999999998</v>
+      </c>
+      <c r="I17" s="5">
+        <v>5.5950000000000001E-8</v>
+      </c>
+      <c r="J17" s="5">
+        <v>4.1300000000000001E-17</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1">
+        <v>12.42846756</v>
+      </c>
+      <c r="E18" s="1">
+        <v>23.54734784</v>
+      </c>
+      <c r="F18" s="1">
+        <v>36.107066189999998</v>
+      </c>
+      <c r="G18" s="1">
+        <v>3.9145545099999999</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>3.5819999999999999E-14</v>
+      </c>
+      <c r="J18" s="5">
+        <v>4.2519999999999996E-28</v>
+      </c>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1">
+        <v>30</v>
+      </c>
+      <c r="E19" s="1">
+        <v>76.634827349999995</v>
+      </c>
+      <c r="F19" s="1">
+        <v>64.102058819999996</v>
+      </c>
+      <c r="G19" s="1">
+        <v>100</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>8.8450000000000002E-13</v>
+      </c>
+      <c r="J19" s="5">
+        <v>2.9759999999999998E-25</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C7DCD5-BDAD-401C-B543-BA34AAEE86EC}">
+  <dimension ref="A3:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="11" max="11" width="17.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>12.74321958</v>
+      </c>
+      <c r="F4" s="1">
+        <v>52.859676589999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>96.838433699999996</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.61568851999999996</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1.1990000000000001E-6</v>
+      </c>
+      <c r="J4" s="5">
+        <v>3.2630000000000002E-14</v>
+      </c>
+      <c r="K4" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1">
+        <v>66.649433500000001</v>
+      </c>
+      <c r="G5" s="1">
+        <v>84.867683600000007</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.02898891E-2</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1.1990000000000001E-6</v>
+      </c>
+      <c r="J5" s="5">
+        <v>3.2630000000000002E-14</v>
+      </c>
+      <c r="K5" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1">
+        <v>17.470003340000002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>12.93364319</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45.791012799999997</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2.2411222899999999</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.52154887000000005</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1.115E-14</v>
+      </c>
+      <c r="J6" s="5">
+        <v>3.2419999999999998E-29</v>
+      </c>
+      <c r="K6" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.0897436200000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>32.140378509999998</v>
+      </c>
+      <c r="F7" s="1">
+        <v>72.052134280000004</v>
+      </c>
+      <c r="G7" s="1">
+        <v>6.6573657500000003</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.37023394999999998</v>
+      </c>
+      <c r="I7" s="5">
+        <v>4.2080000000000002E-14</v>
+      </c>
+      <c r="J7" s="5">
+        <v>3.674E-28</v>
+      </c>
+      <c r="K7" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8" s="1">
+        <v>25.189794970000001</v>
+      </c>
+      <c r="G8" s="1">
+        <v>54.566755100000002</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.59093600999999996</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1.7549999999999999E-6</v>
+      </c>
+      <c r="J8" s="5">
+        <v>5.259E-14</v>
+      </c>
+      <c r="K8" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>30.235382269999999</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>76.554354320000002</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.92326025</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1.7549999999999999E-6</v>
+      </c>
+      <c r="J9" s="5">
+        <v>5.259E-14</v>
+      </c>
+      <c r="K9" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.20799965000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>17.013050060000001</v>
+      </c>
+      <c r="F10" s="1">
+        <v>92.382394430000005</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.9952725299999998</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.37444251000000001</v>
+      </c>
+      <c r="I10" s="5">
+        <v>3.4100000000000001E-14</v>
+      </c>
+      <c r="J10" s="5">
+        <v>3.5590000000000001E-28</v>
+      </c>
+      <c r="K10" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1">
+        <v>17.929191589999999</v>
+      </c>
+      <c r="E11" s="1">
+        <v>69.986283319999998</v>
+      </c>
+      <c r="F11" s="1">
+        <v>35.277896339999998</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2.9669982699999999</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.90833008999999998</v>
+      </c>
+      <c r="I11" s="5">
+        <v>4.3289999999999998E-14</v>
+      </c>
+      <c r="J11" s="5">
+        <v>3.5920000000000001E-28</v>
+      </c>
+      <c r="K11" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>29.42410726</v>
+      </c>
+      <c r="F12" s="1">
+        <v>65.093202829999996</v>
+      </c>
+      <c r="G12" s="1">
+        <v>99.776767070000005</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1.1990000000000001E-6</v>
+      </c>
+      <c r="J12" s="5">
+        <v>3.2630000000000002E-14</v>
+      </c>
+      <c r="K12" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>50.281356850000002</v>
+      </c>
+      <c r="F13" s="1">
+        <v>28.03195152</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2.9069904800000002</v>
+      </c>
+      <c r="H13" s="1">
+        <v>5.0691739999999999E-2</v>
+      </c>
+      <c r="I13" s="5">
+        <v>4.1439999999999999E-8</v>
+      </c>
+      <c r="J13" s="5">
+        <v>5.1279999999999997E-16</v>
+      </c>
+      <c r="K13" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14" s="1">
+        <v>98.218970850000005</v>
+      </c>
+      <c r="G14" s="1">
+        <v>26.76397291</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1.719E-13</v>
+      </c>
+      <c r="J14" s="5">
+        <v>7.9250000000000005E-27</v>
+      </c>
+      <c r="K14" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1">
+        <v>17.179269420000001</v>
+      </c>
+      <c r="E15" s="1">
+        <v>13.20003021</v>
+      </c>
+      <c r="F15" s="1">
+        <v>36.077645130000001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>100</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.41953826999999999</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1.382E-11</v>
+      </c>
+      <c r="J15" s="5">
+        <v>3.4500000000000002E-24</v>
+      </c>
+      <c r="K15" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>97.951985140000005</v>
+      </c>
+      <c r="F16" s="1">
+        <v>41.865225700000003</v>
+      </c>
+      <c r="G16" s="1">
+        <v>59.191153069999999</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.50026252000000004</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1.173E-7</v>
+      </c>
+      <c r="J16" s="5">
+        <v>1.856E-16</v>
+      </c>
+      <c r="K16" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>48.868004130000003</v>
+      </c>
+      <c r="F17" s="1">
+        <v>97.960398749999996</v>
+      </c>
+      <c r="G17" s="1">
+        <v>70.28819627</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.48970525999999998</v>
+      </c>
+      <c r="I17" s="5">
+        <v>5.6050000000000002E-8</v>
+      </c>
+      <c r="J17" s="5">
+        <v>4.1440000000000001E-17</v>
+      </c>
+      <c r="K17" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1">
+        <v>12.42846756</v>
+      </c>
+      <c r="E18" s="1">
+        <v>23.54734784</v>
+      </c>
+      <c r="F18" s="1">
+        <v>36.107066189999998</v>
+      </c>
+      <c r="G18" s="1">
+        <v>3.9145545099999999</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>5.2629999999999999E-14</v>
+      </c>
+      <c r="J18" s="5">
+        <v>4.334E-28</v>
+      </c>
+      <c r="K18" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1">
+        <v>30</v>
+      </c>
+      <c r="E19" s="1">
+        <v>76.634827349999995</v>
+      </c>
+      <c r="F19" s="1">
+        <v>64.102058819999996</v>
+      </c>
+      <c r="G19" s="1">
+        <v>100</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>8.8329999999999998E-13</v>
+      </c>
+      <c r="J19" s="5">
+        <v>2.9769999999999998E-25</v>
+      </c>
+      <c r="K19" s="1">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>